<commit_message>
FMEA: Rechtschreibfehler korrigiert, Warnsymbole herausgesucht
</commit_message>
<xml_diff>
--- a/RB-Blessing/FMEA.xlsx
+++ b/RB-Blessing/FMEA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofmannt.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601AD638-BA4F-475E-9F54-3E7FC0AE4D35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6246B6B-750B-4BB8-AE79-0A9F388460B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" tabRatio="860" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,7 +655,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="339">
   <si>
     <t>1</t>
   </si>
@@ -2155,6 +2155,9 @@
   <si>
     <t>Team: 5620331, 3225750, 1790705, 9269794</t>
   </si>
+  <si>
+    <t>bei Hersteller nach Anwendungstests der Dichtungen erkundigen, Montagewerkzeug zum sachgerechten Anziehen der Dichtungen beilegen</t>
+  </si>
 </sst>
 </file>
 
@@ -3558,7 +3561,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="316">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4203,9 +4206,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -7255,10 +7255,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="12.75" thickBot="1">
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="316"/>
+      <c r="C2" s="315"/>
     </row>
     <row r="3" spans="1:4" ht="33.75" customHeight="1" thickBot="1">
       <c r="A3" s="83" t="s">
@@ -7329,11 +7329,11 @@
     <row r="9" spans="1:4" ht="11.25" customHeight="1" thickBot="1"/>
     <row r="10" spans="1:4" ht="11.25" customHeight="1" thickBot="1">
       <c r="A10" s="82"/>
-      <c r="B10" s="312" t="s">
+      <c r="B10" s="311" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="313"/>
-      <c r="D10" s="314"/>
+      <c r="C10" s="312"/>
+      <c r="D10" s="313"/>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="83" t="s">
@@ -7422,10 +7422,10 @@
     <row r="18" spans="1:3" ht="12.75" thickBot="1"/>
     <row r="19" spans="1:3" ht="12.75" thickBot="1">
       <c r="A19" s="82"/>
-      <c r="B19" s="312" t="s">
+      <c r="B19" s="311" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="314"/>
+      <c r="C19" s="313"/>
     </row>
     <row r="20" spans="1:3" ht="24.75" thickBot="1">
       <c r="A20" s="83" t="s">
@@ -12410,28 +12410,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="74.25" customHeight="1">
-      <c r="B1" s="245"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="247" t="s">
+      <c r="B1" s="244"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="246" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="248"/>
-      <c r="F1" s="248"/>
-      <c r="G1" s="248"/>
-      <c r="H1" s="248"/>
-      <c r="I1" s="248"/>
-      <c r="J1" s="248"/>
-      <c r="K1" s="248"/>
-      <c r="L1" s="248"/>
-      <c r="M1" s="248"/>
-      <c r="N1" s="248"/>
-      <c r="O1" s="248"/>
-      <c r="P1" s="248"/>
-      <c r="Q1" s="248"/>
-      <c r="R1" s="248"/>
-      <c r="S1" s="248"/>
-      <c r="T1" s="248"/>
-      <c r="U1" s="248"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
+      <c r="G1" s="247"/>
+      <c r="H1" s="247"/>
+      <c r="I1" s="247"/>
+      <c r="J1" s="247"/>
+      <c r="K1" s="247"/>
+      <c r="L1" s="247"/>
+      <c r="M1" s="247"/>
+      <c r="N1" s="247"/>
+      <c r="O1" s="247"/>
+      <c r="P1" s="247"/>
+      <c r="Q1" s="247"/>
+      <c r="R1" s="247"/>
+      <c r="S1" s="247"/>
+      <c r="T1" s="247"/>
+      <c r="U1" s="247"/>
       <c r="V1" s="132"/>
     </row>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
@@ -15265,42 +15265,42 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="80.25" customHeight="1">
-      <c r="A3" s="249" t="s">
+      <c r="A3" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="249"/>
-      <c r="C3" s="249"/>
-      <c r="D3" s="249"/>
-      <c r="E3" s="249"/>
-      <c r="F3" s="249"/>
-      <c r="G3" s="249"/>
-      <c r="H3" s="249"/>
-      <c r="I3" s="249"/>
-      <c r="J3" s="249"/>
-      <c r="K3" s="249"/>
-      <c r="L3" s="249"/>
-      <c r="M3" s="249"/>
-      <c r="N3" s="249"/>
-      <c r="O3" s="249"/>
+      <c r="B3" s="248"/>
+      <c r="C3" s="248"/>
+      <c r="D3" s="248"/>
+      <c r="E3" s="248"/>
+      <c r="F3" s="248"/>
+      <c r="G3" s="248"/>
+      <c r="H3" s="248"/>
+      <c r="I3" s="248"/>
+      <c r="J3" s="248"/>
+      <c r="K3" s="248"/>
+      <c r="L3" s="248"/>
+      <c r="M3" s="248"/>
+      <c r="N3" s="248"/>
+      <c r="O3" s="248"/>
     </row>
     <row r="4" spans="1:20" ht="409.5" customHeight="1">
-      <c r="A4" s="249" t="s">
+      <c r="A4" s="248" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="249"/>
-      <c r="C4" s="249"/>
-      <c r="D4" s="249"/>
-      <c r="E4" s="249"/>
-      <c r="F4" s="249"/>
-      <c r="G4" s="249"/>
-      <c r="H4" s="249"/>
-      <c r="I4" s="249"/>
-      <c r="J4" s="249"/>
-      <c r="K4" s="249"/>
-      <c r="L4" s="249"/>
-      <c r="M4" s="249"/>
-      <c r="N4" s="249"/>
-      <c r="O4" s="249"/>
+      <c r="B4" s="248"/>
+      <c r="C4" s="248"/>
+      <c r="D4" s="248"/>
+      <c r="E4" s="248"/>
+      <c r="F4" s="248"/>
+      <c r="G4" s="248"/>
+      <c r="H4" s="248"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="248"/>
+      <c r="K4" s="248"/>
+      <c r="L4" s="248"/>
+      <c r="M4" s="248"/>
+      <c r="N4" s="248"/>
+      <c r="O4" s="248"/>
       <c r="P4" s="224"/>
       <c r="Q4" s="224"/>
       <c r="R4" s="224"/>
@@ -15344,18 +15344,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="75.95" customHeight="1">
-      <c r="A1" s="258"/>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
+      <c r="A1" s="257"/>
+      <c r="B1" s="257"/>
+      <c r="C1" s="257"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257"/>
+      <c r="L1" s="257"/>
       <c r="M1" s="173"/>
       <c r="N1" s="173"/>
       <c r="O1" s="173"/>
@@ -15374,35 +15374,35 @@
     </row>
     <row r="2" spans="1:28" ht="23.25">
       <c r="A2" s="177"/>
-      <c r="B2" s="259" t="s">
+      <c r="B2" s="258" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
-      <c r="J2" s="260"/>
-      <c r="K2" s="260"/>
-      <c r="L2" s="260"/>
-      <c r="M2" s="261"/>
-      <c r="N2" s="262"/>
-      <c r="O2" s="263"/>
-      <c r="P2" s="264" t="s">
+      <c r="C2" s="259"/>
+      <c r="D2" s="259"/>
+      <c r="E2" s="259"/>
+      <c r="F2" s="259"/>
+      <c r="G2" s="259"/>
+      <c r="H2" s="259"/>
+      <c r="I2" s="259"/>
+      <c r="J2" s="259"/>
+      <c r="K2" s="259"/>
+      <c r="L2" s="259"/>
+      <c r="M2" s="260"/>
+      <c r="N2" s="261"/>
+      <c r="O2" s="262"/>
+      <c r="P2" s="263" t="s">
         <v>159</v>
       </c>
-      <c r="Q2" s="265"/>
-      <c r="R2" s="265"/>
-      <c r="S2" s="265"/>
-      <c r="T2" s="265"/>
-      <c r="U2" s="265"/>
-      <c r="V2" s="265"/>
-      <c r="W2" s="265"/>
-      <c r="X2" s="265"/>
-      <c r="Y2" s="265"/>
-      <c r="Z2" s="266"/>
+      <c r="Q2" s="264"/>
+      <c r="R2" s="264"/>
+      <c r="S2" s="264"/>
+      <c r="T2" s="264"/>
+      <c r="U2" s="264"/>
+      <c r="V2" s="264"/>
+      <c r="W2" s="264"/>
+      <c r="X2" s="264"/>
+      <c r="Y2" s="264"/>
+      <c r="Z2" s="265"/>
       <c r="AA2" s="176"/>
     </row>
     <row r="3" spans="1:28" ht="162.94999999999999" customHeight="1">
@@ -15418,22 +15418,22 @@
       <c r="J3" s="201"/>
       <c r="K3" s="201"/>
       <c r="L3" s="201"/>
-      <c r="M3" s="267" t="s">
+      <c r="M3" s="266" t="s">
         <v>154</v>
       </c>
-      <c r="N3" s="267"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="254"/>
-      <c r="Q3" s="252"/>
-      <c r="R3" s="252"/>
-      <c r="S3" s="252"/>
-      <c r="T3" s="252"/>
-      <c r="U3" s="252"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="256"/>
-      <c r="Y3" s="256"/>
-      <c r="Z3" s="256"/>
+      <c r="N3" s="266"/>
+      <c r="O3" s="267"/>
+      <c r="P3" s="253"/>
+      <c r="Q3" s="251"/>
+      <c r="R3" s="251"/>
+      <c r="S3" s="251"/>
+      <c r="T3" s="251"/>
+      <c r="U3" s="251"/>
+      <c r="V3" s="253"/>
+      <c r="W3" s="253"/>
+      <c r="X3" s="255"/>
+      <c r="Y3" s="255"/>
+      <c r="Z3" s="255"/>
       <c r="AA3" s="178"/>
     </row>
     <row r="4" spans="1:28" ht="45">
@@ -15482,23 +15482,23 @@
       <c r="O4" s="181" t="s">
         <v>131</v>
       </c>
-      <c r="P4" s="255"/>
-      <c r="Q4" s="253"/>
-      <c r="R4" s="253"/>
-      <c r="S4" s="253"/>
-      <c r="T4" s="253"/>
-      <c r="U4" s="253"/>
-      <c r="V4" s="255"/>
-      <c r="W4" s="255"/>
-      <c r="X4" s="257"/>
-      <c r="Y4" s="257"/>
-      <c r="Z4" s="257"/>
+      <c r="P4" s="254"/>
+      <c r="Q4" s="252"/>
+      <c r="R4" s="252"/>
+      <c r="S4" s="252"/>
+      <c r="T4" s="252"/>
+      <c r="U4" s="252"/>
+      <c r="V4" s="254"/>
+      <c r="W4" s="254"/>
+      <c r="X4" s="256"/>
+      <c r="Y4" s="256"/>
+      <c r="Z4" s="256"/>
       <c r="AA4" s="181" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A5" s="250" t="s">
+      <c r="A5" s="249" t="s">
         <v>132</v>
       </c>
       <c r="B5" s="182"/>
@@ -15536,12 +15536,12 @@
         <f>SUM(P5:W5)</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="250" t="s">
+      <c r="AB5" s="249" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A6" s="251"/>
+      <c r="A6" s="250"/>
       <c r="B6" s="189"/>
       <c r="C6" s="189"/>
       <c r="D6" s="189"/>
@@ -15577,10 +15577,10 @@
         <f t="shared" ref="AA6:AA14" si="2">SUM(P6:W6)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="251"/>
+      <c r="AB6" s="250"/>
     </row>
     <row r="7" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A7" s="251"/>
+      <c r="A7" s="250"/>
       <c r="B7" s="189"/>
       <c r="C7" s="189"/>
       <c r="D7" s="189"/>
@@ -15616,10 +15616,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="251"/>
+      <c r="AB7" s="250"/>
     </row>
     <row r="8" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A8" s="251"/>
+      <c r="A8" s="250"/>
       <c r="B8" s="182"/>
       <c r="C8" s="182"/>
       <c r="D8" s="182"/>
@@ -15655,10 +15655,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB8" s="251"/>
+      <c r="AB8" s="250"/>
     </row>
     <row r="9" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A9" s="251"/>
+      <c r="A9" s="250"/>
       <c r="B9" s="182"/>
       <c r="C9" s="182"/>
       <c r="D9" s="182"/>
@@ -15694,10 +15694,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="251"/>
+      <c r="AB9" s="250"/>
     </row>
     <row r="10" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A10" s="251"/>
+      <c r="A10" s="250"/>
       <c r="B10" s="182"/>
       <c r="C10" s="182"/>
       <c r="D10" s="182"/>
@@ -15733,10 +15733,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="251"/>
+      <c r="AB10" s="250"/>
     </row>
     <row r="11" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A11" s="251"/>
+      <c r="A11" s="250"/>
       <c r="B11" s="189"/>
       <c r="C11" s="189"/>
       <c r="D11" s="189"/>
@@ -15772,10 +15772,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="251"/>
+      <c r="AB11" s="250"/>
     </row>
     <row r="12" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A12" s="251"/>
+      <c r="A12" s="250"/>
       <c r="B12" s="182"/>
       <c r="C12" s="182"/>
       <c r="D12" s="182"/>
@@ -15811,10 +15811,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB12" s="251"/>
+      <c r="AB12" s="250"/>
     </row>
     <row r="13" spans="1:28" ht="22.5" customHeight="1">
-      <c r="A13" s="251"/>
+      <c r="A13" s="250"/>
       <c r="B13" s="189"/>
       <c r="C13" s="182"/>
       <c r="D13" s="182"/>
@@ -15850,10 +15850,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB13" s="251"/>
+      <c r="AB13" s="250"/>
     </row>
     <row r="14" spans="1:28" ht="23.25">
-      <c r="A14" s="251"/>
+      <c r="A14" s="250"/>
       <c r="B14" s="182"/>
       <c r="C14" s="182"/>
       <c r="D14" s="182"/>
@@ -15889,7 +15889,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="251"/>
+      <c r="AB14" s="250"/>
     </row>
     <row r="15" spans="1:28">
       <c r="A15" s="180" t="s">
@@ -16302,9 +16302,9 @@
   </sheetPr>
   <dimension ref="A1:AD162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -16334,36 +16334,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="D1" s="272" t="s">
+      <c r="D1" s="271" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="274" t="s">
+      <c r="E1" s="273" t="s">
         <v>289</v>
       </c>
       <c r="F1" s="95" t="s">
         <v>337</v>
       </c>
-      <c r="G1" s="280" t="s">
+      <c r="G1" s="279" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="281"/>
-      <c r="M1" s="281"/>
-      <c r="N1" s="281"/>
-      <c r="O1" s="281"/>
-      <c r="P1" s="281"/>
-      <c r="Q1" s="281"/>
-      <c r="R1" s="281"/>
-      <c r="S1" s="281"/>
-      <c r="T1" s="281"/>
-      <c r="U1" s="281"/>
-      <c r="V1" s="281"/>
-      <c r="W1" s="281"/>
-      <c r="X1" s="281"/>
-      <c r="Y1" s="282"/>
+      <c r="H1" s="280"/>
+      <c r="I1" s="280"/>
+      <c r="J1" s="280"/>
+      <c r="K1" s="280"/>
+      <c r="L1" s="280"/>
+      <c r="M1" s="280"/>
+      <c r="N1" s="280"/>
+      <c r="O1" s="280"/>
+      <c r="P1" s="280"/>
+      <c r="Q1" s="280"/>
+      <c r="R1" s="280"/>
+      <c r="S1" s="280"/>
+      <c r="T1" s="280"/>
+      <c r="U1" s="280"/>
+      <c r="V1" s="280"/>
+      <c r="W1" s="280"/>
+      <c r="X1" s="280"/>
+      <c r="Y1" s="281"/>
       <c r="AA1" s="78">
         <v>1</v>
       </c>
@@ -16378,28 +16378,28 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="D2" s="273"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="269"/>
-      <c r="G2" s="283"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="284"/>
-      <c r="J2" s="284"/>
-      <c r="K2" s="284"/>
-      <c r="L2" s="284"/>
-      <c r="M2" s="284"/>
-      <c r="N2" s="284"/>
-      <c r="O2" s="284"/>
-      <c r="P2" s="284"/>
-      <c r="Q2" s="284"/>
-      <c r="R2" s="284"/>
-      <c r="S2" s="284"/>
-      <c r="T2" s="284"/>
-      <c r="U2" s="284"/>
-      <c r="V2" s="284"/>
-      <c r="W2" s="284"/>
-      <c r="X2" s="284"/>
-      <c r="Y2" s="285"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="274"/>
+      <c r="F2" s="268"/>
+      <c r="G2" s="282"/>
+      <c r="H2" s="283"/>
+      <c r="I2" s="283"/>
+      <c r="J2" s="283"/>
+      <c r="K2" s="283"/>
+      <c r="L2" s="283"/>
+      <c r="M2" s="283"/>
+      <c r="N2" s="283"/>
+      <c r="O2" s="283"/>
+      <c r="P2" s="283"/>
+      <c r="Q2" s="283"/>
+      <c r="R2" s="283"/>
+      <c r="S2" s="283"/>
+      <c r="T2" s="283"/>
+      <c r="U2" s="283"/>
+      <c r="V2" s="283"/>
+      <c r="W2" s="283"/>
+      <c r="X2" s="283"/>
+      <c r="Y2" s="284"/>
       <c r="AA2" s="78">
         <v>2</v>
       </c>
@@ -16414,28 +16414,28 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="D3" s="273"/>
-      <c r="E3" s="276"/>
-      <c r="F3" s="269"/>
-      <c r="G3" s="283"/>
-      <c r="H3" s="284"/>
-      <c r="I3" s="284"/>
-      <c r="J3" s="284"/>
-      <c r="K3" s="284"/>
-      <c r="L3" s="284"/>
-      <c r="M3" s="284"/>
-      <c r="N3" s="284"/>
-      <c r="O3" s="284"/>
-      <c r="P3" s="284"/>
-      <c r="Q3" s="284"/>
-      <c r="R3" s="284"/>
-      <c r="S3" s="284"/>
-      <c r="T3" s="284"/>
-      <c r="U3" s="284"/>
-      <c r="V3" s="284"/>
-      <c r="W3" s="284"/>
-      <c r="X3" s="284"/>
-      <c r="Y3" s="285"/>
+      <c r="D3" s="272"/>
+      <c r="E3" s="275"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="282"/>
+      <c r="H3" s="283"/>
+      <c r="I3" s="283"/>
+      <c r="J3" s="283"/>
+      <c r="K3" s="283"/>
+      <c r="L3" s="283"/>
+      <c r="M3" s="283"/>
+      <c r="N3" s="283"/>
+      <c r="O3" s="283"/>
+      <c r="P3" s="283"/>
+      <c r="Q3" s="283"/>
+      <c r="R3" s="283"/>
+      <c r="S3" s="283"/>
+      <c r="T3" s="283"/>
+      <c r="U3" s="283"/>
+      <c r="V3" s="283"/>
+      <c r="W3" s="283"/>
+      <c r="X3" s="283"/>
+      <c r="Y3" s="284"/>
       <c r="AA3" s="78">
         <v>3</v>
       </c>
@@ -16447,102 +16447,102 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="D4" s="272" t="s">
+      <c r="D4" s="271" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="277">
+      <c r="E4" s="276">
         <f ca="1">TODAY()</f>
         <v>43798</v>
       </c>
-      <c r="F4" s="269"/>
-      <c r="G4" s="283"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284"/>
-      <c r="J4" s="284"/>
-      <c r="K4" s="284"/>
-      <c r="L4" s="284"/>
-      <c r="M4" s="284"/>
-      <c r="N4" s="284"/>
-      <c r="O4" s="284"/>
-      <c r="P4" s="284"/>
-      <c r="Q4" s="284"/>
-      <c r="R4" s="284"/>
-      <c r="S4" s="284"/>
-      <c r="T4" s="284"/>
-      <c r="U4" s="284"/>
-      <c r="V4" s="284"/>
-      <c r="W4" s="284"/>
-      <c r="X4" s="284"/>
-      <c r="Y4" s="285"/>
+      <c r="F4" s="268"/>
+      <c r="G4" s="282"/>
+      <c r="H4" s="283"/>
+      <c r="I4" s="283"/>
+      <c r="J4" s="283"/>
+      <c r="K4" s="283"/>
+      <c r="L4" s="283"/>
+      <c r="M4" s="283"/>
+      <c r="N4" s="283"/>
+      <c r="O4" s="283"/>
+      <c r="P4" s="283"/>
+      <c r="Q4" s="283"/>
+      <c r="R4" s="283"/>
+      <c r="S4" s="283"/>
+      <c r="T4" s="283"/>
+      <c r="U4" s="283"/>
+      <c r="V4" s="283"/>
+      <c r="W4" s="283"/>
+      <c r="X4" s="283"/>
+      <c r="Y4" s="284"/>
       <c r="AA4" s="78">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="D5" s="273"/>
-      <c r="E5" s="278"/>
-      <c r="F5" s="269"/>
-      <c r="G5" s="283"/>
-      <c r="H5" s="284"/>
-      <c r="I5" s="284"/>
-      <c r="J5" s="284"/>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
-      <c r="M5" s="284"/>
-      <c r="N5" s="284"/>
-      <c r="O5" s="284"/>
-      <c r="P5" s="284"/>
-      <c r="Q5" s="284"/>
-      <c r="R5" s="284"/>
-      <c r="S5" s="284"/>
-      <c r="T5" s="284"/>
-      <c r="U5" s="284"/>
-      <c r="V5" s="284"/>
-      <c r="W5" s="284"/>
-      <c r="X5" s="284"/>
-      <c r="Y5" s="285"/>
+      <c r="D5" s="272"/>
+      <c r="E5" s="277"/>
+      <c r="F5" s="268"/>
+      <c r="G5" s="282"/>
+      <c r="H5" s="283"/>
+      <c r="I5" s="283"/>
+      <c r="J5" s="283"/>
+      <c r="K5" s="283"/>
+      <c r="L5" s="283"/>
+      <c r="M5" s="283"/>
+      <c r="N5" s="283"/>
+      <c r="O5" s="283"/>
+      <c r="P5" s="283"/>
+      <c r="Q5" s="283"/>
+      <c r="R5" s="283"/>
+      <c r="S5" s="283"/>
+      <c r="T5" s="283"/>
+      <c r="U5" s="283"/>
+      <c r="V5" s="283"/>
+      <c r="W5" s="283"/>
+      <c r="X5" s="283"/>
+      <c r="Y5" s="284"/>
       <c r="AA5" s="78">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="14.25" customHeight="1" outlineLevel="1" thickBot="1">
-      <c r="D6" s="273"/>
-      <c r="E6" s="279"/>
-      <c r="F6" s="270"/>
-      <c r="G6" s="283"/>
-      <c r="H6" s="284"/>
-      <c r="I6" s="284"/>
-      <c r="J6" s="284"/>
-      <c r="K6" s="284"/>
-      <c r="L6" s="284"/>
-      <c r="M6" s="284"/>
-      <c r="N6" s="284"/>
-      <c r="O6" s="284"/>
-      <c r="P6" s="284"/>
-      <c r="Q6" s="284"/>
-      <c r="R6" s="284"/>
-      <c r="S6" s="284"/>
-      <c r="T6" s="284"/>
-      <c r="U6" s="284"/>
-      <c r="V6" s="284"/>
-      <c r="W6" s="284"/>
-      <c r="X6" s="284"/>
-      <c r="Y6" s="285"/>
+      <c r="D6" s="272"/>
+      <c r="E6" s="278"/>
+      <c r="F6" s="269"/>
+      <c r="G6" s="282"/>
+      <c r="H6" s="283"/>
+      <c r="I6" s="283"/>
+      <c r="J6" s="283"/>
+      <c r="K6" s="283"/>
+      <c r="L6" s="283"/>
+      <c r="M6" s="283"/>
+      <c r="N6" s="283"/>
+      <c r="O6" s="283"/>
+      <c r="P6" s="283"/>
+      <c r="Q6" s="283"/>
+      <c r="R6" s="283"/>
+      <c r="S6" s="283"/>
+      <c r="T6" s="283"/>
+      <c r="U6" s="283"/>
+      <c r="V6" s="283"/>
+      <c r="W6" s="283"/>
+      <c r="X6" s="283"/>
+      <c r="Y6" s="284"/>
       <c r="AA6" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="3" customFormat="1" ht="45">
-      <c r="D7" s="298" t="s">
+      <c r="D7" s="297" t="s">
         <v>179</v>
       </c>
-      <c r="E7" s="288" t="s">
+      <c r="E7" s="287" t="s">
         <v>180</v>
       </c>
-      <c r="F7" s="288" t="s">
+      <c r="F7" s="287" t="s">
         <v>181</v>
       </c>
-      <c r="G7" s="288" t="s">
+      <c r="G7" s="287" t="s">
         <v>270</v>
       </c>
       <c r="H7" s="29" t="s">
@@ -16560,43 +16560,43 @@
       <c r="L7" s="76" t="s">
         <v>306</v>
       </c>
-      <c r="M7" s="290" t="s">
+      <c r="M7" s="289" t="s">
         <v>183</v>
       </c>
-      <c r="N7" s="286" t="s">
+      <c r="N7" s="285" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="286" t="s">
+      <c r="O7" s="285" t="s">
         <v>335</v>
       </c>
-      <c r="P7" s="294" t="s">
+      <c r="P7" s="293" t="s">
         <v>336</v>
       </c>
-      <c r="Q7" s="296" t="s">
+      <c r="Q7" s="295" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="297" t="s">
+      <c r="R7" s="296" t="s">
         <v>88</v>
       </c>
-      <c r="S7" s="292" t="s">
+      <c r="S7" s="291" t="s">
         <v>161</v>
       </c>
-      <c r="T7" s="292" t="s">
+      <c r="T7" s="291" t="s">
         <v>162</v>
       </c>
-      <c r="U7" s="292" t="s">
+      <c r="U7" s="291" t="s">
         <v>163</v>
       </c>
-      <c r="V7" s="271" t="s">
+      <c r="V7" s="270" t="s">
         <v>87</v>
       </c>
-      <c r="W7" s="293" t="s">
+      <c r="W7" s="292" t="s">
         <v>164</v>
       </c>
-      <c r="X7" s="293" t="s">
+      <c r="X7" s="292" t="s">
         <v>165</v>
       </c>
-      <c r="Y7" s="293" t="s">
+      <c r="Y7" s="292" t="s">
         <v>166</v>
       </c>
       <c r="AA7" s="3">
@@ -16604,10 +16604,10 @@
       </c>
     </row>
     <row r="8" spans="1:30" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="D8" s="299"/>
-      <c r="E8" s="289"/>
-      <c r="F8" s="289"/>
-      <c r="G8" s="289"/>
+      <c r="D8" s="298"/>
+      <c r="E8" s="288"/>
+      <c r="F8" s="288"/>
+      <c r="G8" s="288"/>
       <c r="H8" s="29" t="s">
         <v>2</v>
       </c>
@@ -16623,19 +16623,19 @@
       <c r="L8" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="291"/>
-      <c r="N8" s="287"/>
-      <c r="O8" s="287"/>
-      <c r="P8" s="295"/>
-      <c r="Q8" s="296"/>
-      <c r="R8" s="297"/>
-      <c r="S8" s="292"/>
-      <c r="T8" s="292"/>
-      <c r="U8" s="292"/>
-      <c r="V8" s="271"/>
-      <c r="W8" s="293"/>
-      <c r="X8" s="293"/>
-      <c r="Y8" s="293"/>
+      <c r="M8" s="290"/>
+      <c r="N8" s="286"/>
+      <c r="O8" s="286"/>
+      <c r="P8" s="294"/>
+      <c r="Q8" s="295"/>
+      <c r="R8" s="296"/>
+      <c r="S8" s="291"/>
+      <c r="T8" s="291"/>
+      <c r="U8" s="291"/>
+      <c r="V8" s="270"/>
+      <c r="W8" s="292"/>
+      <c r="X8" s="292"/>
+      <c r="Y8" s="292"/>
       <c r="AA8" s="3">
         <v>8</v>
       </c>
@@ -16958,8 +16958,8 @@
         <f>IFERROR(VLOOKUP(CONCATENATE(H14,I14,J14),'Task Priority (TP)'!$P:$Q,2,FALSE),"")</f>
         <v>H</v>
       </c>
-      <c r="M14" s="243" t="s">
-        <v>280</v>
+      <c r="M14" s="242" t="s">
+        <v>338</v>
       </c>
       <c r="N14" s="21">
         <v>10</v>
@@ -17029,7 +17029,7 @@
         <f>IFERROR(VLOOKUP(CONCATENATE(H15,I15,J15),'Task Priority (TP)'!$P:$Q,2,FALSE),"")</f>
         <v>H</v>
       </c>
-      <c r="M15" s="243" t="s">
+      <c r="M15" s="242" t="s">
         <v>281</v>
       </c>
       <c r="N15" s="21">
@@ -17100,7 +17100,7 @@
         <f>IFERROR(VLOOKUP(CONCATENATE(H16,I16,J16),'Task Priority (TP)'!$P:$Q,2,FALSE),"")</f>
         <v>H</v>
       </c>
-      <c r="M16" s="243" t="s">
+      <c r="M16" s="242" t="s">
         <v>282</v>
       </c>
       <c r="N16" s="21">
@@ -17171,7 +17171,7 @@
         <f>IFERROR(VLOOKUP(CONCATENATE(H17,I17,J17),'Task Priority (TP)'!$P:$Q,2,FALSE),"")</f>
         <v>H</v>
       </c>
-      <c r="M17" s="243" t="s">
+      <c r="M17" s="242" t="s">
         <v>283</v>
       </c>
       <c r="N17" s="21">
@@ -17219,7 +17219,7 @@
       <c r="E18" s="239" t="s">
         <v>198</v>
       </c>
-      <c r="F18" s="242" t="s">
+      <c r="F18" s="241" t="s">
         <v>264</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -17242,7 +17242,7 @@
         <f>IFERROR(VLOOKUP(CONCATENATE(H18,I18,J18),'Task Priority (TP)'!$P:$Q,2,FALSE),"")</f>
         <v>M</v>
       </c>
-      <c r="M18" s="243" t="s">
+      <c r="M18" s="242" t="s">
         <v>326</v>
       </c>
       <c r="N18" s="21">
@@ -18526,7 +18526,7 @@
       <c r="D38" s="239" t="s">
         <v>227</v>
       </c>
-      <c r="E38" s="241" t="s">
+      <c r="E38" s="243" t="s">
         <v>234</v>
       </c>
       <c r="F38" s="239" t="s">
@@ -18597,7 +18597,7 @@
       <c r="D39" s="239" t="s">
         <v>227</v>
       </c>
-      <c r="E39" s="241" t="s">
+      <c r="E39" s="243" t="s">
         <v>234</v>
       </c>
       <c r="F39" s="239" t="s">
@@ -20004,7 +20004,7 @@
         <f>IFERROR(VLOOKUP(CONCATENATE(H60,I60,J60),'Task Priority (TP)'!$P:$Q,2,FALSE),"")</f>
         <v>H</v>
       </c>
-      <c r="M60" s="243" t="s">
+      <c r="M60" s="242" t="s">
         <v>280</v>
       </c>
       <c r="N60" s="21">
@@ -20117,7 +20117,7 @@
       <c r="C62" s="90">
         <v>53</v>
       </c>
-      <c r="D62" s="244" t="s">
+      <c r="D62" s="243" t="s">
         <v>297</v>
       </c>
       <c r="E62" s="239" t="s">
@@ -20178,7 +20178,7 @@
       <c r="C63" s="90">
         <v>54</v>
       </c>
-      <c r="D63" s="244" t="s">
+      <c r="D63" s="243" t="s">
         <v>297</v>
       </c>
       <c r="E63" s="239" t="s">
@@ -20237,7 +20237,7 @@
         <v>5.5000000000000003E-8</v>
       </c>
       <c r="C64" s="90"/>
-      <c r="D64" s="244"/>
+      <c r="D64" s="243"/>
       <c r="E64" s="239"/>
       <c r="F64" s="239"/>
       <c r="G64" s="2" t="s">
@@ -20284,7 +20284,7 @@
         <v>5.6000000000000005E-8</v>
       </c>
       <c r="C65" s="90"/>
-      <c r="D65" s="244"/>
+      <c r="D65" s="243"/>
       <c r="E65" s="239"/>
       <c r="F65" s="239"/>
       <c r="G65" s="2" t="s">
@@ -24902,11 +24902,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="B1" s="300"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="302"/>
+      <c r="B1" s="299"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="301"/>
       <c r="G1" s="31"/>
       <c r="H1" s="31">
         <f>'[2]FMEA_system_sub-system_comp-1'!D1:Q1</f>
@@ -24914,11 +24914,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="B2" s="303"/>
-      <c r="C2" s="304"/>
-      <c r="D2" s="304"/>
-      <c r="E2" s="304"/>
-      <c r="F2" s="305"/>
+      <c r="B2" s="302"/>
+      <c r="C2" s="303"/>
+      <c r="D2" s="303"/>
+      <c r="E2" s="303"/>
+      <c r="F2" s="304"/>
       <c r="G2" s="33" t="s">
         <v>26</v>
       </c>
@@ -24928,23 +24928,23 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="47.1" customHeight="1">
-      <c r="B3" s="306"/>
-      <c r="C3" s="307"/>
-      <c r="D3" s="307"/>
-      <c r="E3" s="307"/>
-      <c r="F3" s="308"/>
+      <c r="B3" s="305"/>
+      <c r="C3" s="306"/>
+      <c r="D3" s="306"/>
+      <c r="E3" s="306"/>
+      <c r="F3" s="307"/>
       <c r="G3" s="35"/>
       <c r="H3" s="35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="37" customFormat="1" ht="11.25">
-      <c r="B4" s="309"/>
-      <c r="C4" s="310"/>
-      <c r="D4" s="311"/>
-      <c r="E4" s="311"/>
-      <c r="F4" s="311"/>
-      <c r="G4" s="311"/>
+      <c r="B4" s="308"/>
+      <c r="C4" s="309"/>
+      <c r="D4" s="310"/>
+      <c r="E4" s="310"/>
+      <c r="F4" s="310"/>
+      <c r="G4" s="310"/>
       <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8">

</xml_diff>